<commit_message>
Voy a cambiar X y Y, empezando ha hacer la documentacion
</commit_message>
<xml_diff>
--- a/Practicas/Practica 2/Tablas.xlsx
+++ b/Practicas/Practica 2/Tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Escritorio\Universidad\Cuarto año\Primer cuatri\SI\Practicas\Practica 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B044AF-6255-4291-80C0-B7B69E2EECB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79799C58-68FD-4A92-B183-ABAB122BBB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A1:AH62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>